<commit_message>
antes dos testes da reuniao 26/08
</commit_message>
<xml_diff>
--- a/backend/cmd/simulation/consumo_diario.xlsx
+++ b/backend/cmd/simulation/consumo_diario.xlsx
@@ -378,25 +378,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4544</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>5.88</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>13104</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>35858.28</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>8.15</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>53520.310000000005</v>
       </c>
     </row>
     <row r="3">
@@ -404,25 +404,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4736</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>39.36</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>43.65</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>10224</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>35468.67</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>50511.67999999999</v>
       </c>
     </row>
     <row r="4">
@@ -430,25 +430,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4862</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>871.79</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>919.58</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10800</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>35693.31</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>81.67</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>53228.34999999999</v>
       </c>
     </row>
     <row r="5">
@@ -456,25 +456,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>7236</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10591.85</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>12151.5</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>14256</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>42595.48</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>2431.5</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>89262.33</v>
       </c>
     </row>
     <row r="6">
@@ -482,25 +482,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>18398</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>52350.26</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>62941.53</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>51984</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>101223.82</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>24516.14</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>311413.75</v>
       </c>
     </row>
     <row r="7">
@@ -508,25 +508,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>37016</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>114924.91</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>131737.7</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>149472</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>296065.26</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>119522.57</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>848738.44</v>
       </c>
     </row>
     <row r="8">
@@ -534,25 +534,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>64970</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>254796.6</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>246824.99</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>310896</v>
       </c>
       <c r="F8">
-        <v>1.26</v>
+        <v>577702.4</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>287319.94</v>
       </c>
       <c r="H8">
-        <v>1.26</v>
+        <v>1742509.93</v>
       </c>
     </row>
     <row r="9">
@@ -560,25 +560,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>71652</v>
       </c>
       <c r="C9">
-        <v>15.48</v>
+        <v>366853.63</v>
       </c>
       <c r="D9">
-        <v>1.59</v>
+        <v>317068.5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>232704</v>
       </c>
       <c r="F9">
-        <v>2.09</v>
+        <v>430127.94</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>175900.63</v>
       </c>
       <c r="H9">
-        <v>19.16</v>
+        <v>1594306.7000000002</v>
       </c>
     </row>
     <row r="10">
@@ -586,25 +586,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>18942</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>83955.49</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>80286.24</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>67680</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>108885.49</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>41099.06</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>400848.28</v>
       </c>
     </row>
     <row r="11">
@@ -612,25 +612,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>9676</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>34554.29</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>34860.74</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>42048</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>63945.23</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>25182.49</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>210266.75</v>
       </c>
     </row>
     <row r="12">
@@ -638,25 +638,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>7524</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>24203.62</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>26909.73</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>26928</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>45729.61</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>15694.42</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>146989.38000000003</v>
       </c>
     </row>
     <row r="13">
@@ -664,25 +664,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>11090</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>40971.58</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>50641.16</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>23760</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>41391.22</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>8783.19</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>176637.15000000002</v>
       </c>
     </row>
     <row r="14">
@@ -690,25 +690,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>20524</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>71516.91</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>113937.47</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>31824</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>54037.38</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>4531.6</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>296371.36</v>
       </c>
     </row>
     <row r="15">
@@ -716,25 +716,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>28966</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>59819.23</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>155077.26</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>40896</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>96901.17</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>2208.43</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>383868.08999999997</v>
       </c>
     </row>
     <row r="16">
@@ -742,25 +742,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>35200</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>66494.81</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>154748.2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>75456</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>183380.68</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1340.87</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>516620.56</v>
       </c>
     </row>
     <row r="17">
@@ -768,25 +768,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>46912</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>90214.77</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>172740.33</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>129168</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>309365.09</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>532.26</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>748932.45</v>
       </c>
     </row>
     <row r="18">
@@ -794,25 +794,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>57282</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>118517.95</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>153137.12</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>175104</v>
       </c>
       <c r="F18">
-        <v>8.78</v>
+        <v>452247.29</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>105.84</v>
       </c>
       <c r="H18">
-        <v>8.78</v>
+        <v>956394.2</v>
       </c>
     </row>
     <row r="19">
@@ -820,25 +820,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>64190</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>140877.81</v>
       </c>
       <c r="D19">
-        <v>3.6</v>
+        <v>120788.95</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>232992</v>
       </c>
       <c r="F19">
-        <v>5.1</v>
+        <v>589716.82</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>9.65</v>
       </c>
       <c r="H19">
-        <v>8.7</v>
+        <v>1148575.23</v>
       </c>
     </row>
     <row r="20">
@@ -846,25 +846,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>74316</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>234079.1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>142299.29</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>259920</v>
       </c>
       <c r="F20">
-        <v>2.16</v>
+        <v>663277.97</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>27.62</v>
       </c>
       <c r="H20">
-        <v>2.16</v>
+        <v>1373919.98</v>
       </c>
     </row>
     <row r="21">
@@ -872,25 +872,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>70850</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>191141.86</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>123446.99</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>251856</v>
       </c>
       <c r="F21">
-        <v>5.87</v>
+        <v>655664.5</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>5.87</v>
+        <v>1292959.35</v>
       </c>
     </row>
     <row r="22">
@@ -898,25 +898,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>61274</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>130059.08</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>116683.37</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>212544</v>
       </c>
       <c r="F22">
-        <v>5.19</v>
+        <v>573511.06</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>5.19</v>
+        <v>1094071.51</v>
       </c>
     </row>
     <row r="23">
@@ -924,25 +924,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>51730</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>103329.06</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>152569.41</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>174528</v>
       </c>
       <c r="F23">
-        <v>12.25</v>
+        <v>433865.24</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>12.25</v>
+        <v>916021.71</v>
       </c>
     </row>
     <row r="24">
@@ -950,25 +950,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>37356</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>71781.4</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>131021.31</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>105120</v>
       </c>
       <c r="F24">
-        <v>2.81</v>
+        <v>264276.29</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>2.81</v>
+        <v>609555</v>
       </c>
     </row>
     <row r="25">
@@ -976,25 +976,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>23744</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>43613.81</v>
       </c>
       <c r="D25">
-        <v>5.88</v>
+        <v>98595.26</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>59328</v>
       </c>
       <c r="F25">
-        <v>0.74</v>
+        <v>136454.52</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>6.62</v>
+        <v>361735.58999999997</v>
       </c>
     </row>
     <row r="26">
@@ -1002,25 +1002,25 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>832990</v>
       </c>
       <c r="C26">
-        <v>15.48</v>
+        <v>2305559.1700000004</v>
       </c>
       <c r="D26">
-        <v>11.07</v>
+        <v>2599436.16</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>2702592</v>
       </c>
       <c r="F26">
-        <v>46.25000000000001</v>
+        <v>6227384.72</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>709296.0299999999</v>
       </c>
       <c r="H26">
-        <v>72.80000000000001</v>
+        <v>15377258.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimo comit antes de terminar o backend
</commit_message>
<xml_diff>
--- a/backend/cmd/simulation/consumo_diario.xlsx
+++ b/backend/cmd/simulation/consumo_diario.xlsx
@@ -378,25 +378,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4544</v>
+        <v>22498.56</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>5.88</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>13104</v>
+        <v>11520</v>
       </c>
       <c r="F2">
-        <v>35858.28</v>
+        <v>16910.97</v>
       </c>
       <c r="G2">
-        <v>8.15</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>53520.310000000005</v>
+        <v>50929.53</v>
       </c>
     </row>
     <row r="3">
@@ -404,25 +404,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4736</v>
+        <v>21985.99</v>
       </c>
       <c r="C3">
-        <v>39.36</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>43.65</v>
+        <v>30.79</v>
       </c>
       <c r="E3">
-        <v>10224</v>
+        <v>13248</v>
       </c>
       <c r="F3">
-        <v>35468.67</v>
+        <v>16540.65</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>50511.67999999999</v>
+        <v>51805.43</v>
       </c>
     </row>
     <row r="4">
@@ -430,25 +430,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4862</v>
+        <v>23854.82</v>
       </c>
       <c r="C4">
-        <v>871.79</v>
+        <v>2323.9</v>
       </c>
       <c r="D4">
-        <v>919.58</v>
+        <v>693.4</v>
       </c>
       <c r="E4">
-        <v>10800</v>
+        <v>11952</v>
       </c>
       <c r="F4">
-        <v>35693.31</v>
+        <v>16854.9</v>
       </c>
       <c r="G4">
-        <v>81.67</v>
+        <v>185.97</v>
       </c>
       <c r="H4">
-        <v>53228.34999999999</v>
+        <v>55864.990000000005</v>
       </c>
     </row>
     <row r="5">
@@ -456,25 +456,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7236</v>
+        <v>35485.13</v>
       </c>
       <c r="C5">
-        <v>10591.85</v>
+        <v>25914.59</v>
       </c>
       <c r="D5">
-        <v>12151.5</v>
+        <v>8216.36</v>
       </c>
       <c r="E5">
-        <v>14256</v>
+        <v>15552</v>
       </c>
       <c r="F5">
-        <v>42595.48</v>
+        <v>20551.35</v>
       </c>
       <c r="G5">
-        <v>2431.5</v>
+        <v>2687.62</v>
       </c>
       <c r="H5">
-        <v>89262.33</v>
+        <v>108407.04999999999</v>
       </c>
     </row>
     <row r="6">
@@ -482,25 +482,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>18398</v>
+        <v>87036.77</v>
       </c>
       <c r="C6">
-        <v>52350.26</v>
+        <v>135940.31</v>
       </c>
       <c r="D6">
-        <v>62941.53</v>
+        <v>42676.89</v>
       </c>
       <c r="E6">
-        <v>51984</v>
+        <v>50688</v>
       </c>
       <c r="F6">
-        <v>101223.82</v>
+        <v>48075.07</v>
       </c>
       <c r="G6">
-        <v>24516.14</v>
+        <v>23981.08</v>
       </c>
       <c r="H6">
-        <v>311413.75</v>
+        <v>388398.12000000005</v>
       </c>
     </row>
     <row r="7">
@@ -508,25 +508,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>37016</v>
+        <v>174123.43</v>
       </c>
       <c r="C7">
-        <v>114924.91</v>
+        <v>294064.14</v>
       </c>
       <c r="D7">
-        <v>131737.7</v>
+        <v>91546.6</v>
       </c>
       <c r="E7">
-        <v>149472</v>
+        <v>165312</v>
       </c>
       <c r="F7">
-        <v>296065.26</v>
+        <v>140757.72</v>
       </c>
       <c r="G7">
-        <v>119522.57</v>
+        <v>119035.97</v>
       </c>
       <c r="H7">
-        <v>848738.44</v>
+        <v>984839.86</v>
       </c>
     </row>
     <row r="8">
@@ -534,25 +534,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>64970</v>
+        <v>309196.44</v>
       </c>
       <c r="C8">
-        <v>254796.6</v>
+        <v>637007.94</v>
       </c>
       <c r="D8">
-        <v>246824.99</v>
+        <v>169399.69</v>
       </c>
       <c r="E8">
-        <v>310896</v>
+        <v>319968</v>
       </c>
       <c r="F8">
-        <v>577702.4</v>
+        <v>275531.02</v>
       </c>
       <c r="G8">
-        <v>287319.94</v>
+        <v>289989.18</v>
       </c>
       <c r="H8">
-        <v>1742509.93</v>
+        <v>2001092.2699999998</v>
       </c>
     </row>
     <row r="9">
@@ -560,25 +560,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>71652</v>
+        <v>342077.9</v>
       </c>
       <c r="C9">
-        <v>366853.63</v>
+        <v>919414</v>
       </c>
       <c r="D9">
-        <v>317068.5</v>
+        <v>219039.01</v>
       </c>
       <c r="E9">
-        <v>232704</v>
+        <v>236160</v>
       </c>
       <c r="F9">
-        <v>430127.94</v>
+        <v>202643.26</v>
       </c>
       <c r="G9">
-        <v>175900.63</v>
+        <v>175946.06</v>
       </c>
       <c r="H9">
-        <v>1594306.7000000002</v>
+        <v>2095280.23</v>
       </c>
     </row>
     <row r="10">
@@ -586,25 +586,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>18942</v>
+        <v>91173.6</v>
       </c>
       <c r="C10">
-        <v>83955.49</v>
+        <v>213868.43</v>
       </c>
       <c r="D10">
-        <v>80286.24</v>
+        <v>55604.07</v>
       </c>
       <c r="E10">
-        <v>67680</v>
+        <v>66384</v>
       </c>
       <c r="F10">
-        <v>108885.49</v>
+        <v>51454.45</v>
       </c>
       <c r="G10">
-        <v>41099.06</v>
+        <v>41025.91</v>
       </c>
       <c r="H10">
-        <v>400848.28</v>
+        <v>519510.4600000001</v>
       </c>
     </row>
     <row r="11">
@@ -612,25 +612,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>9676</v>
+        <v>45477.94</v>
       </c>
       <c r="C11">
-        <v>34554.29</v>
+        <v>83172.57</v>
       </c>
       <c r="D11">
-        <v>34860.74</v>
+        <v>23725.63</v>
       </c>
       <c r="E11">
-        <v>42048</v>
+        <v>42768</v>
       </c>
       <c r="F11">
-        <v>63945.23</v>
+        <v>29809.51</v>
       </c>
       <c r="G11">
-        <v>25182.49</v>
+        <v>25275.5</v>
       </c>
       <c r="H11">
-        <v>210266.75</v>
+        <v>250229.15000000002</v>
       </c>
     </row>
     <row r="12">
@@ -638,25 +638,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>7524</v>
+        <v>35290.08</v>
       </c>
       <c r="C12">
-        <v>24203.62</v>
+        <v>58541.06</v>
       </c>
       <c r="D12">
-        <v>26909.73</v>
+        <v>19032.29</v>
       </c>
       <c r="E12">
-        <v>26928</v>
+        <v>29376</v>
       </c>
       <c r="F12">
-        <v>45729.61</v>
+        <v>21597.93</v>
       </c>
       <c r="G12">
-        <v>15694.42</v>
+        <v>15357.05</v>
       </c>
       <c r="H12">
-        <v>146989.38000000003</v>
+        <v>179194.40999999997</v>
       </c>
     </row>
     <row r="13">
@@ -664,25 +664,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>11090</v>
+        <v>51451.85</v>
       </c>
       <c r="C13">
-        <v>40971.58</v>
+        <v>98694.22</v>
       </c>
       <c r="D13">
-        <v>50641.16</v>
+        <v>34182.15</v>
       </c>
       <c r="E13">
-        <v>23760</v>
+        <v>28656</v>
       </c>
       <c r="F13">
-        <v>41391.22</v>
+        <v>19262.13</v>
       </c>
       <c r="G13">
-        <v>8783.19</v>
+        <v>8777.88</v>
       </c>
       <c r="H13">
-        <v>176637.15000000002</v>
+        <v>241024.23</v>
       </c>
     </row>
     <row r="14">
@@ -690,25 +690,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>20524</v>
+        <v>97605.65</v>
       </c>
       <c r="C14">
-        <v>71516.91</v>
+        <v>172450.76</v>
       </c>
       <c r="D14">
-        <v>113937.47</v>
+        <v>79397.75</v>
       </c>
       <c r="E14">
-        <v>31824</v>
+        <v>30240</v>
       </c>
       <c r="F14">
-        <v>54037.38</v>
+        <v>25785.34</v>
       </c>
       <c r="G14">
-        <v>4531.6</v>
+        <v>4772.27</v>
       </c>
       <c r="H14">
-        <v>296371.36</v>
+        <v>410251.7700000001</v>
       </c>
     </row>
     <row r="15">
@@ -716,25 +716,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>28966</v>
+        <v>138452.33</v>
       </c>
       <c r="C15">
-        <v>59819.23</v>
+        <v>152199.9</v>
       </c>
       <c r="D15">
-        <v>155077.26</v>
+        <v>109267.26</v>
       </c>
       <c r="E15">
-        <v>40896</v>
+        <v>44352</v>
       </c>
       <c r="F15">
-        <v>96901.17</v>
+        <v>46375.51</v>
       </c>
       <c r="G15">
-        <v>2208.43</v>
+        <v>2412.73</v>
       </c>
       <c r="H15">
-        <v>383868.08999999997</v>
+        <v>493059.73</v>
       </c>
     </row>
     <row r="16">
@@ -742,25 +742,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>35200</v>
+        <v>169718.98</v>
       </c>
       <c r="C16">
-        <v>66494.81</v>
+        <v>165781.06</v>
       </c>
       <c r="D16">
-        <v>154748.2</v>
+        <v>104992.97</v>
       </c>
       <c r="E16">
-        <v>75456</v>
+        <v>82512</v>
       </c>
       <c r="F16">
-        <v>183380.68</v>
+        <v>87610</v>
       </c>
       <c r="G16">
-        <v>1340.87</v>
+        <v>906.99</v>
       </c>
       <c r="H16">
-        <v>516620.56</v>
+        <v>611522</v>
       </c>
     </row>
     <row r="17">
@@ -768,25 +768,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>46912</v>
+        <v>225856.51</v>
       </c>
       <c r="C17">
-        <v>90214.77</v>
+        <v>228133.64</v>
       </c>
       <c r="D17">
-        <v>172740.33</v>
+        <v>116714.5</v>
       </c>
       <c r="E17">
-        <v>129168</v>
+        <v>124848</v>
       </c>
       <c r="F17">
-        <v>309365.09</v>
+        <v>148030.49</v>
       </c>
       <c r="G17">
-        <v>532.26</v>
+        <v>447.45</v>
       </c>
       <c r="H17">
-        <v>748932.45</v>
+        <v>844030.59</v>
       </c>
     </row>
     <row r="18">
@@ -794,25 +794,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>57282</v>
+        <v>272785.97</v>
       </c>
       <c r="C18">
-        <v>118517.95</v>
+        <v>292342.57</v>
       </c>
       <c r="D18">
-        <v>153137.12</v>
+        <v>105406.58</v>
       </c>
       <c r="E18">
-        <v>175104</v>
+        <v>181296</v>
       </c>
       <c r="F18">
-        <v>452247.29</v>
+        <v>219152.19</v>
       </c>
       <c r="G18">
-        <v>105.84</v>
+        <v>83.2</v>
       </c>
       <c r="H18">
-        <v>956394.2</v>
+        <v>1071066.51</v>
       </c>
     </row>
     <row r="19">
@@ -820,25 +820,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>64190</v>
+        <v>304320.24</v>
       </c>
       <c r="C19">
-        <v>140877.81</v>
+        <v>345825.14</v>
       </c>
       <c r="D19">
-        <v>120788.95</v>
+        <v>80827.76</v>
       </c>
       <c r="E19">
-        <v>232992</v>
+        <v>233568</v>
       </c>
       <c r="F19">
-        <v>589716.82</v>
+        <v>279286.04</v>
       </c>
       <c r="G19">
-        <v>9.65</v>
+        <v>43.95</v>
       </c>
       <c r="H19">
-        <v>1148575.23</v>
+        <v>1243871.13</v>
       </c>
     </row>
     <row r="20">
@@ -846,25 +846,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>74316</v>
+        <v>347711.62</v>
       </c>
       <c r="C20">
-        <v>234079.1</v>
+        <v>584450.36</v>
       </c>
       <c r="D20">
-        <v>142299.29</v>
+        <v>97618.75</v>
       </c>
       <c r="E20">
-        <v>259920</v>
+        <v>260640</v>
       </c>
       <c r="F20">
-        <v>663277.97</v>
+        <v>315581.01</v>
       </c>
       <c r="G20">
-        <v>27.62</v>
+        <v>2.84</v>
       </c>
       <c r="H20">
-        <v>1373919.98</v>
+        <v>1606004.58</v>
       </c>
     </row>
     <row r="21">
@@ -872,25 +872,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>70850</v>
+        <v>336031.42</v>
       </c>
       <c r="C21">
-        <v>191141.86</v>
+        <v>476414.17</v>
       </c>
       <c r="D21">
-        <v>123446.99</v>
+        <v>84929.69</v>
       </c>
       <c r="E21">
-        <v>251856</v>
+        <v>259344</v>
       </c>
       <c r="F21">
-        <v>655664.5</v>
+        <v>310325.02</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1292959.35</v>
+        <v>1467044.3</v>
       </c>
     </row>
     <row r="22">
@@ -898,25 +898,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>61274</v>
+        <v>291007.08</v>
       </c>
       <c r="C22">
-        <v>130059.08</v>
+        <v>328205.12</v>
       </c>
       <c r="D22">
-        <v>116683.37</v>
+        <v>79629.07</v>
       </c>
       <c r="E22">
-        <v>212544</v>
+        <v>215136</v>
       </c>
       <c r="F22">
-        <v>573511.06</v>
+        <v>272284.27</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H22">
-        <v>1094071.51</v>
+        <v>1186267.79</v>
       </c>
     </row>
     <row r="23">
@@ -924,25 +924,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>51730</v>
+        <v>248119.2</v>
       </c>
       <c r="C23">
-        <v>103329.06</v>
+        <v>271564.83</v>
       </c>
       <c r="D23">
-        <v>152569.41</v>
+        <v>106462.05</v>
       </c>
       <c r="E23">
-        <v>174528</v>
+        <v>175968</v>
       </c>
       <c r="F23">
-        <v>433865.24</v>
+        <v>206664.28</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>916021.71</v>
+        <v>1008778.3600000001</v>
       </c>
     </row>
     <row r="24">
@@ -950,25 +950,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>37356</v>
+        <v>174486.31</v>
       </c>
       <c r="C24">
-        <v>71781.4</v>
+        <v>181982.86</v>
       </c>
       <c r="D24">
-        <v>131021.31</v>
+        <v>88774.3</v>
       </c>
       <c r="E24">
-        <v>105120</v>
+        <v>112032</v>
       </c>
       <c r="F24">
-        <v>264276.29</v>
+        <v>125266.81</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>609555</v>
+        <v>682542.28</v>
       </c>
     </row>
     <row r="25">
@@ -976,25 +976,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>23744</v>
+        <v>112628.88</v>
       </c>
       <c r="C25">
-        <v>43613.81</v>
+        <v>111315.81</v>
       </c>
       <c r="D25">
-        <v>98595.26</v>
+        <v>66530.67</v>
       </c>
       <c r="E25">
-        <v>59328</v>
+        <v>62784</v>
       </c>
       <c r="F25">
-        <v>136454.52</v>
+        <v>62623.86</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>361735.58999999997</v>
+        <v>415883.22</v>
       </c>
     </row>
     <row r="26">
@@ -1002,25 +1002,25 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>832990</v>
+        <v>3958376.7000000007</v>
       </c>
       <c r="C26">
-        <v>2305559.1700000004</v>
+        <v>5779607.38</v>
       </c>
       <c r="D26">
-        <v>2599436.16</v>
+        <v>1784698.23</v>
       </c>
       <c r="E26">
-        <v>2702592</v>
+        <v>2774304</v>
       </c>
       <c r="F26">
-        <v>6227384.72</v>
+        <v>2958973.78</v>
       </c>
       <c r="G26">
-        <v>709296.0299999999</v>
+        <v>710937.8999999999</v>
       </c>
       <c r="H26">
-        <v>15377258.08</v>
+        <v>17966897.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>